<commit_message>
Astrophysics and thermo couple updates
</commit_message>
<xml_diff>
--- a/Thermo-couple/temp.xlsx
+++ b/Thermo-couple/temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>T[C]</t>
   </si>
@@ -27,16 +27,13 @@
   <si>
     <t>ΔV</t>
   </si>
-  <si>
-    <t/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +44,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -78,18 +81,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -403,10 +403,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -423,244 +423,298 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2">
-        <v>6.592</v>
+        <v>87.475</v>
       </c>
       <c r="B2" s="2">
         <v>0.054</v>
       </c>
       <c r="C2" s="2">
-        <v>0.22</v>
+        <v>3.7</v>
       </c>
       <c r="D2" s="2">
-        <v>0.020066</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+        <v>0.02111</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2">
-        <v>-4.96</v>
+        <v>82.108</v>
       </c>
       <c r="B3" s="2">
         <v>0.054</v>
       </c>
       <c r="C3" s="2">
-        <v>-0.21</v>
+        <v>3.44</v>
       </c>
       <c r="D3" s="2">
-        <v>0.019937</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+        <v>0.021032</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2">
-        <v>-19.067</v>
+        <v>76.708</v>
       </c>
       <c r="B4" s="2">
         <v>0.054</v>
       </c>
       <c r="C4" s="2">
-        <v>-0.77</v>
+        <v>3.18</v>
       </c>
       <c r="D4" s="2">
-        <v>0.019769</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+        <v>0.020954</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2">
-        <v>-25.93</v>
+        <v>72.3</v>
       </c>
       <c r="B5" s="2">
         <v>0.054</v>
       </c>
       <c r="C5" s="2">
-        <v>-1.02</v>
+        <v>2.97</v>
       </c>
       <c r="D5" s="2">
-        <v>0.019694</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+        <v>0.020891</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2">
-        <v>-32.045</v>
+        <v>69.008</v>
       </c>
       <c r="B6" s="2">
         <v>0.054</v>
       </c>
       <c r="C6" s="2">
-        <v>-1.25</v>
+        <v>2.81</v>
       </c>
       <c r="D6" s="2">
-        <v>0.019625</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+        <v>0.020843</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2">
-        <v>-41.675</v>
+        <v>64.217</v>
       </c>
       <c r="B7" s="2">
         <v>0.054</v>
       </c>
       <c r="C7" s="2">
-        <v>-1.6</v>
+        <v>2.69</v>
       </c>
       <c r="D7" s="2">
-        <v>0.01952</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+        <v>0.020807</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2">
-        <v>-49.079</v>
+        <v>55.51</v>
       </c>
       <c r="B8" s="2">
         <v>0.05</v>
       </c>
       <c r="C8" s="2">
-        <v>-1.88</v>
+        <v>2.59</v>
       </c>
       <c r="D8" s="2">
-        <v>0.019436</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+        <v>0.020777</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2">
-        <v>-58.533</v>
+        <v>51.33</v>
       </c>
       <c r="B9" s="2">
         <v>0.05</v>
       </c>
       <c r="C9" s="2">
-        <v>-2.26</v>
+        <v>2.49</v>
       </c>
       <c r="D9" s="2">
-        <v>0.019322</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+        <v>0.020747</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="2">
-        <v>-73.217</v>
+        <v>48.36</v>
       </c>
       <c r="B10" s="2">
         <v>0.05</v>
       </c>
       <c r="C10" s="2">
-        <v>-2.69</v>
+        <v>2.39</v>
       </c>
       <c r="D10" s="2">
-        <v>0.019193</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+        <v>0.020717</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="2">
-        <v>-79.633</v>
+        <v>48.74</v>
       </c>
       <c r="B11" s="2">
         <v>0.05</v>
       </c>
       <c r="C11" s="2">
-        <v>-2.91</v>
+        <v>2.25</v>
       </c>
       <c r="D11" s="2">
-        <v>0.019127</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+        <v>0.020675</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="2">
-        <v>-87.457</v>
+        <v>46.84</v>
       </c>
       <c r="B12" s="2">
         <v>0.05</v>
       </c>
       <c r="C12" s="2">
-        <v>-3.18</v>
+        <v>2.08</v>
       </c>
       <c r="D12" s="2">
-        <v>0.019046</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+        <v>0.020624</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="2">
-        <v>-96.58</v>
+        <v>44.56</v>
       </c>
       <c r="B13" s="2">
         <v>0.05</v>
       </c>
       <c r="C13" s="2">
-        <v>-3.47</v>
+        <v>1.87</v>
       </c>
       <c r="D13" s="2">
-        <v>0.018959</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+        <v>0.020561</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="2">
-        <v>-104.24</v>
+        <v>40.76</v>
       </c>
       <c r="B14" s="2">
         <v>0.05</v>
       </c>
       <c r="C14" s="2">
-        <v>-3.65</v>
+        <v>1.7</v>
       </c>
       <c r="D14" s="2">
-        <v>0.018905</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="4" t="s">
-        <v>4</v>
+        <v>0.02051</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="2">
+        <v>37.533</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.054</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.02048</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="2">
+        <v>33.013</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.020408</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="2">
+        <v>28.287</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.02033</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="2">
+        <v>25.65</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.0203</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="2">
+        <v>24.332</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.020285</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="2">
+        <v>23.39</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.020276</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="2">
+        <v>17.72</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.020207</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="2">
+        <v>7.533</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.020072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>